<commit_message>
Rettede alle SLKs lkommentarer igennem plus basecamp.
</commit_message>
<xml_diff>
--- a/data/data_varmefylde.xlsx
+++ b/data/data_varmefylde.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16416" windowHeight="6792"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18240" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -215,6 +215,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -326,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -341,6 +345,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,22 +632,22 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.8203125" defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="6.3125" customWidth="1"/>
-    <col min="2" max="2" width="32.3125" customWidth="1"/>
-    <col min="3" max="3" width="19.15625" customWidth="1"/>
-    <col min="4" max="4" width="13.734375" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="31.5234375" customWidth="1"/>
-    <col min="8" max="8" width="13.20703125" customWidth="1"/>
+    <col min="1" max="1" width="6.29296875" customWidth="1"/>
+    <col min="2" max="2" width="32.29296875" customWidth="1"/>
+    <col min="3" max="3" width="19.17578125" customWidth="1"/>
+    <col min="4" max="4" width="13.703125" customWidth="1"/>
+    <col min="6" max="6" width="8.8203125" customWidth="1"/>
+    <col min="7" max="7" width="31.52734375" customWidth="1"/>
+    <col min="8" max="8" width="13.17578125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="33.299999999999997">
+    <row r="1" spans="1:17" ht="33.35">
       <c r="A1" s="1"/>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -683,12 +691,14 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" ht="27.3">
+    <row r="3" spans="1:17" ht="26.7">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>0.1012</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
@@ -712,12 +722,14 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" ht="27.3">
+    <row r="4" spans="1:17" ht="26.7">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="13">
+        <v>0.14599999999999999</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
@@ -741,7 +753,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:17" ht="23.1">
+    <row r="5" spans="1:17" ht="23.35">
       <c r="A5" s="1"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -766,12 +778,14 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="27.3">
+    <row r="6" spans="1:17" ht="27">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="9">
+        <v>22.6</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
@@ -795,7 +809,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="27.3">
+    <row r="7" spans="1:17" ht="26.7">
       <c r="A7" s="1"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
@@ -820,12 +834,14 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="1:17" ht="27.3">
+    <row r="8" spans="1:17" ht="26.7">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="12">
+        <v>32</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
@@ -862,7 +878,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="1:17" ht="29.4" customHeight="1">
+    <row r="10" spans="1:17" ht="29.45" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>4</v>

</xml_diff>